<commit_message>
launch 2024 class website
</commit_message>
<xml_diff>
--- a/data/syllabus650.xlsx
+++ b/data/syllabus650.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daviddl\Documents\EDLD 650\EDLD 650\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADCA0B2-3571-4BDB-8149-3202A454E71D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Topics</t>
   </si>
@@ -59,9 +60,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>MM Ch. 9 &lt;br&gt; [Angrist &amp; Lavy 1999](https://doi.org/10.1162/003355399556061) &lt;br&gt; [Ludwig &amp; Miller 2007](https://doi.org/10.1162/qjec.122.1.159)</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -125,76 +123,82 @@
     <t>MM Ch. 13 &amp; 14 &lt;br&gt; [Umansky &amp; Dumont 2021](https://doi.org/10.3102%2F0002831221997571)</t>
   </si>
   <si>
-    <t>A Common Vocabulary</t>
-  </si>
-  <si>
     <t>[Liebowitz et al. 2021](https://doi.org/10.1080/19345747.2021.2015496)</t>
   </si>
   <si>
     <t>Class Date</t>
   </si>
   <si>
-    <t>Jan. 4</t>
-  </si>
-  <si>
-    <t>Jan. 11</t>
-  </si>
-  <si>
-    <t>Jan. 18</t>
-  </si>
-  <si>
-    <t>Jan. 25</t>
-  </si>
-  <si>
-    <t>Feb. 1</t>
-  </si>
-  <si>
-    <t>Feb. 8</t>
-  </si>
-  <si>
-    <t>Feb. 15</t>
-  </si>
-  <si>
-    <t>Feb. 22</t>
-  </si>
-  <si>
-    <t>Mar. 1</t>
-  </si>
-  <si>
-    <t>Mar. 8</t>
-  </si>
-  <si>
     <t>Assignments Due</t>
   </si>
   <si>
-    <t>Student survey (Jan. 5)</t>
-  </si>
-  <si>
-    <t>DARE #1 (Jan. 17)</t>
-  </si>
-  <si>
     <t>Research project proposal (Jan. 28)</t>
   </si>
   <si>
-    <t>DARE #2 (Jan. 31)</t>
-  </si>
-  <si>
-    <t>DARE #3 (Feb. 14)</t>
-  </si>
-  <si>
-    <t>DARE #4 (Feb. 28)</t>
-  </si>
-  <si>
-    <t>Research project presentation (Mar. 8)</t>
-  </si>
-  <si>
-    <t>Final research project (Mar. 17)</t>
+    <t>Student survey (Jan. 10)</t>
+  </si>
+  <si>
+    <t>Jan. 8</t>
+  </si>
+  <si>
+    <t>Jan. 22</t>
+  </si>
+  <si>
+    <t>Jan. 29</t>
+  </si>
+  <si>
+    <t>Feb. 5</t>
+  </si>
+  <si>
+    <t>Feb. 12</t>
+  </si>
+  <si>
+    <t>Feb. 19</t>
+  </si>
+  <si>
+    <t>Feb. 26</t>
+  </si>
+  <si>
+    <t>Mar. 4</t>
+  </si>
+  <si>
+    <t>Mar. 11</t>
+  </si>
+  <si>
+    <t>DARE #1 (Jan. 21)</t>
+  </si>
+  <si>
+    <t>DARE #2 (Feb. 5)</t>
+  </si>
+  <si>
+    <t>DARE #3 (Feb. 18)</t>
+  </si>
+  <si>
+    <t>DARE #4 (Mar. 3)</t>
+  </si>
+  <si>
+    <t>Research project presentation (Mar. 11)</t>
+  </si>
+  <si>
+    <t>Final research project (Mar. 20)</t>
+  </si>
+  <si>
+    <t>MM Ch. 9 &lt;br&gt; [Angrist &amp; Lavy 1999](https://doi.org/10.1162/003355399556061) &lt;br&gt; [Dee &amp; Penner 2017](https://journals.sagepub.com/doi/full/10.3102/0002831216677002)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Common Vocabulary                                    </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,11 +228,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,11 +510,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,10 +529,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -539,7 +541,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -547,16 +549,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>47</v>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,15 +566,15 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -584,13 +586,13 @@
         <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -601,80 +603,80 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>50</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>51</v>
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -686,13 +688,13 @@
         <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -703,28 +705,30 @@
         <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>20</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>54</v>
+      <c r="E12" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>